<commit_message>
something working but results not accurate
</commit_message>
<xml_diff>
--- a/precision_3.xlsx
+++ b/precision_3.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,38 +476,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.395735890226014e-08</v>
+        <v>0.2412331314783636</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0001189794216909371</v>
+        <v>522.7384330412233</v>
       </c>
       <c r="E2" t="n">
-        <v>3.070435708463215e-08</v>
+        <v>0.1567800643885285</v>
       </c>
       <c r="F2" t="n">
-        <v>3.817826221708477e-06</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>torch.float16</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0001562392855883055</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.3664942845114626</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0001105731646042496</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.2134822189615418</v>
+        <v>187.2378100545062</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,38 +549,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.496870961843798e-09</v>
+        <v>0.0112197145813409</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0001386081538551262</v>
+        <v>1524.443749419503</v>
       </c>
       <c r="E2" t="n">
-        <v>6.079660481647653e-10</v>
+        <v>0.005926851996257251</v>
       </c>
       <c r="F2" t="n">
-        <v>9.984561183847128e-05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>torch.float16</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1.070374246414174e-05</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6437158982772805</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3.000312877046176e-06</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.2838328791583394</v>
+        <v>469.8066630824756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CUEQ workinggit add .!
</commit_message>
<xml_diff>
--- a/precision_3.xlsx
+++ b/precision_3.xlsx
@@ -476,16 +476,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2412331314783636</v>
+        <v>3.315138836796488e-08</v>
       </c>
       <c r="D2" t="n">
-        <v>522.7384330412233</v>
+        <v>0.001253061629053576</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1567800643885285</v>
+        <v>1.726506744514911e-08</v>
       </c>
       <c r="F2" t="n">
-        <v>187.2378100545062</v>
+        <v>2.260962129280777e-05</v>
       </c>
     </row>
   </sheetData>
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0112197145813409</v>
+        <v>2.311383758869801e-09</v>
       </c>
       <c r="D2" t="n">
-        <v>1524.443749419503</v>
+        <v>0.005861695524878178</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005926851996257251</v>
+        <v>1.329795547982959e-09</v>
       </c>
       <c r="F2" t="n">
-        <v>469.8066630824756</v>
+        <v>0.0001357465553551715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>